<commit_message>
update as of 2024/05/02
update as of 2024/05/02
</commit_message>
<xml_diff>
--- a/company_list.xlsx
+++ b/company_list.xlsx
@@ -5,20 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Laptop-ssaa9d9q\d\tao_project\valuation_engine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\GitHub\hellotaoworld\valuation_engine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7BFD079-72BF-4FA4-B3DE-3FD07CBA985C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3E3E2E-1655-4F29-BC0E-981936AA1E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{B82EAC9A-0CE0-46BB-ACD0-5E3D12938F59}"/>
+    <workbookView xWindow="31725" yWindow="0" windowWidth="24780" windowHeight="15735" activeTab="2" xr2:uid="{B82EAC9A-0CE0-46BB-ACD0-5E3D12938F59}"/>
   </bookViews>
   <sheets>
     <sheet name="sic" sheetId="3" r:id="rId1"/>
     <sheet name="sp500" sheetId="1" r:id="rId2"/>
     <sheet name="pick" sheetId="2" r:id="rId3"/>
+    <sheet name="checked_pick" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">pick!$A$1:$C$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">pick!$A$1:$C$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">sic!$A$1:$C$445</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'sp500'!$A$1:$G$504</definedName>
   </definedNames>
@@ -89,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3498" uniqueCount="1906">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3607" uniqueCount="1982">
   <si>
     <t>symbol</t>
   </si>
@@ -5807,6 +5808,234 @@
   </si>
   <si>
     <t>SOUNDHOUND AI, INC.</t>
+  </si>
+  <si>
+    <t>GENERAL ELECTRIC CO</t>
+  </si>
+  <si>
+    <t>BOEING CO</t>
+  </si>
+  <si>
+    <t>Uber Technologies, Inc</t>
+  </si>
+  <si>
+    <t>GWH</t>
+  </si>
+  <si>
+    <t>ESS Tech, Inc.</t>
+  </si>
+  <si>
+    <t>ALBEMARLE CORP</t>
+  </si>
+  <si>
+    <t>RIVN</t>
+  </si>
+  <si>
+    <t>Rivian Automotive, Inc.</t>
+  </si>
+  <si>
+    <t>FIRST SOLAR, INC.</t>
+  </si>
+  <si>
+    <t>EXXON MOBIL CORP</t>
+  </si>
+  <si>
+    <t>CHEVRON CORP</t>
+  </si>
+  <si>
+    <t>LCID</t>
+  </si>
+  <si>
+    <t>Lucid Group, Inc.</t>
+  </si>
+  <si>
+    <t>MCDONALDS CORP</t>
+  </si>
+  <si>
+    <t>FEDEX CORP</t>
+  </si>
+  <si>
+    <t>Affirm Holdings, Inc.</t>
+  </si>
+  <si>
+    <t>AFRM</t>
+  </si>
+  <si>
+    <t>HOME DEPOT, INC.</t>
+  </si>
+  <si>
+    <t>AMAZON COM INC</t>
+  </si>
+  <si>
+    <t>3M CO</t>
+  </si>
+  <si>
+    <t>Salesforce, Inc.</t>
+  </si>
+  <si>
+    <t>MICROSOFT CORP</t>
+  </si>
+  <si>
+    <t>ADOBE INC.</t>
+  </si>
+  <si>
+    <t>COSTCO WHOLESALE CORP</t>
+  </si>
+  <si>
+    <t>Walt Disney Co</t>
+  </si>
+  <si>
+    <t>CATERPILLAR INC</t>
+  </si>
+  <si>
+    <t>TEAM</t>
+  </si>
+  <si>
+    <t>Atlassian Corp</t>
+  </si>
+  <si>
+    <t>QUALCOMM INC</t>
+  </si>
+  <si>
+    <t>Walmart Inc.</t>
+  </si>
+  <si>
+    <t>VISA INC.</t>
+  </si>
+  <si>
+    <t>SQ</t>
+  </si>
+  <si>
+    <t>Block, Inc.</t>
+  </si>
+  <si>
+    <t>EOG RESOURCES INC</t>
+  </si>
+  <si>
+    <t>Marathon Petroleum Corp</t>
+  </si>
+  <si>
+    <t>PIONEER NATURAL RESOURCES CO</t>
+  </si>
+  <si>
+    <t>HORTON D R INC</t>
+  </si>
+  <si>
+    <t>LNG</t>
+  </si>
+  <si>
+    <t>Cheniere Energy, Inc.</t>
+  </si>
+  <si>
+    <t>CQP</t>
+  </si>
+  <si>
+    <t>Cheniere Energy Partners, L.P.</t>
+  </si>
+  <si>
+    <t>FCNCA</t>
+  </si>
+  <si>
+    <t>FIRST CITIZENS BANCSHARES INC</t>
+  </si>
+  <si>
+    <t>STEEL DYNAMICS INC</t>
+  </si>
+  <si>
+    <t>CF Industries Holdings, Inc.</t>
+  </si>
+  <si>
+    <t>ATKR</t>
+  </si>
+  <si>
+    <t>Atkore Inc.</t>
+  </si>
+  <si>
+    <t>PBF</t>
+  </si>
+  <si>
+    <t>PBF Energy Inc.</t>
+  </si>
+  <si>
+    <t>LNTH</t>
+  </si>
+  <si>
+    <t>Lantheus Holdings, Inc.</t>
+  </si>
+  <si>
+    <t>WIRE</t>
+  </si>
+  <si>
+    <t>ENCORE WIRE CORP</t>
+  </si>
+  <si>
+    <t>ACLS</t>
+  </si>
+  <si>
+    <t>AXCELIS TECHNOLOGIES INC</t>
+  </si>
+  <si>
+    <t>CNX</t>
+  </si>
+  <si>
+    <t>CNX Resources Corp</t>
+  </si>
+  <si>
+    <t>AX</t>
+  </si>
+  <si>
+    <t>Axos Financial, Inc.</t>
+  </si>
+  <si>
+    <t>CALM</t>
+  </si>
+  <si>
+    <t>CAL-MAINE FOODS INC</t>
+  </si>
+  <si>
+    <t>GRBK</t>
+  </si>
+  <si>
+    <t>Green Brick Partners, Inc.</t>
+  </si>
+  <si>
+    <t>TGLS</t>
+  </si>
+  <si>
+    <t>Tecnoglass Inc.</t>
+  </si>
+  <si>
+    <t>CEIX</t>
+  </si>
+  <si>
+    <t>CONSOL Energy Inc.</t>
+  </si>
+  <si>
+    <t>PARR</t>
+  </si>
+  <si>
+    <t>PAR PACIFIC HOLDINGS, INC.</t>
+  </si>
+  <si>
+    <t>DDD</t>
+  </si>
+  <si>
+    <t>3D SYSTEMS CORP</t>
+  </si>
+  <si>
+    <t>PLUG</t>
+  </si>
+  <si>
+    <t>PLUG POWER INC</t>
+  </si>
+  <si>
+    <t>Enphase Energy, Inc.</t>
+  </si>
+  <si>
+    <t>PLTR</t>
+  </si>
+  <si>
+    <t>Palantir Technologies Inc.</t>
   </si>
 </sst>
 </file>
@@ -11234,7 +11463,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DB4D047-C06A-42FE-BFF0-99FF6773CE7A}">
   <dimension ref="A1:G504"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -22848,10 +23079,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17146AA1-C78E-482C-A866-46B8415D9924}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22873,219 +23107,827 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>2488</v>
+        <v>821189</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>562</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>1939</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>4127</v>
+        <v>1510295</v>
       </c>
       <c r="B3" t="s">
-        <v>1218</v>
+        <v>916</v>
       </c>
       <c r="C3" t="s">
-        <v>1219</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>6281</v>
+        <v>1038357</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>1116</v>
       </c>
       <c r="C4" t="s">
-        <v>147</v>
+        <v>1941</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>6951</v>
+        <v>882184</v>
       </c>
       <c r="B5" t="s">
-        <v>166</v>
+        <v>516</v>
       </c>
       <c r="C5" t="s">
-        <v>167</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>50863</v>
+        <v>3570</v>
       </c>
       <c r="B6" t="s">
-        <v>777</v>
+        <v>1943</v>
       </c>
       <c r="C6" t="s">
-        <v>778</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>97476</v>
+        <v>1383650</v>
       </c>
       <c r="B7" t="s">
-        <v>1277</v>
+        <v>1945</v>
       </c>
       <c r="C7" t="s">
-        <v>1278</v>
+        <v>1946</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>103730</v>
+        <v>798941</v>
       </c>
       <c r="B8" t="s">
-        <v>1436</v>
+        <v>1947</v>
       </c>
       <c r="C8" t="s">
-        <v>1438</v>
+        <v>1948</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>106040</v>
+        <v>1022671</v>
       </c>
       <c r="B9" t="s">
-        <v>1396</v>
+        <v>1237</v>
       </c>
       <c r="C9" t="s">
-        <v>1397</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>319201</v>
+        <v>1324404</v>
       </c>
       <c r="B10" t="s">
-        <v>855</v>
+        <v>348</v>
       </c>
       <c r="C10" t="s">
-        <v>856</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>707549</v>
+        <v>1666138</v>
       </c>
       <c r="B11" t="s">
-        <v>873</v>
+        <v>1951</v>
       </c>
       <c r="C11" t="s">
-        <v>874</v>
+        <v>1952</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>723125</v>
+        <v>1534504</v>
       </c>
       <c r="B12" t="s">
-        <v>964</v>
+        <v>1953</v>
       </c>
       <c r="C12" t="s">
-        <v>965</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>827054</v>
+        <v>1521036</v>
       </c>
       <c r="B13" t="s">
-        <v>961</v>
+        <v>1955</v>
       </c>
       <c r="C13" t="s">
-        <v>962</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>1045810</v>
+        <v>850460</v>
       </c>
       <c r="B14" t="s">
-        <v>1051</v>
+        <v>1957</v>
       </c>
       <c r="C14" t="s">
-        <v>1052</v>
+        <v>1958</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15">
-        <v>1047127</v>
+        <v>1113232</v>
       </c>
       <c r="B15" t="s">
-        <v>1433</v>
+        <v>1959</v>
       </c>
       <c r="C15" t="s">
-        <v>1437</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <v>1097864</v>
+        <v>1070412</v>
       </c>
       <c r="B16" t="s">
-        <v>1068</v>
+        <v>1961</v>
       </c>
       <c r="C16" t="s">
-        <v>1069</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17">
-        <v>1101302</v>
+        <v>1299709</v>
       </c>
       <c r="B17" t="s">
-        <v>1435</v>
+        <v>1963</v>
       </c>
       <c r="C17" t="s">
-        <v>1434</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18">
-        <v>1375365</v>
+        <v>16160</v>
       </c>
       <c r="B18" t="s">
-        <v>1440</v>
+        <v>1965</v>
       </c>
       <c r="C18" t="s">
-        <v>1439</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>1730168</v>
+        <v>1373670</v>
       </c>
       <c r="B19" t="s">
-        <v>274</v>
+        <v>1967</v>
       </c>
       <c r="C19" t="s">
-        <v>275</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
+        <v>1534675</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1969</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>1710366</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1971</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1972</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>821483</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1973</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1974</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>910638</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1975</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1976</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>1093691</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1977</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1978</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>1463101</v>
+      </c>
+      <c r="B25" t="s">
+        <v>556</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1979</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <v>1321655</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1980</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27">
+        <v>1045810</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28">
+        <v>1047127</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1433</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29">
+        <v>1097864</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30">
+        <v>1101302</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31">
+        <v>1375365</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1440</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32">
+        <v>1730168</v>
+      </c>
+      <c r="B32" t="s">
+        <v>274</v>
+      </c>
+      <c r="C32" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33">
         <v>1840856</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B33" t="s">
         <v>1904</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C33" t="s">
         <v>1905</v>
       </c>
     </row>
+    <row r="34" spans="1:3">
+      <c r="A34">
+        <v>40545</v>
+      </c>
+      <c r="B34" t="s">
+        <v>678</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1906</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35">
+        <v>12927</v>
+      </c>
+      <c r="B35" t="s">
+        <v>257</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1907</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36">
+        <v>1543151</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1310</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1908</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37">
+        <v>2488</v>
+      </c>
+      <c r="B37" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38">
+        <v>4127</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1219</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39">
+        <v>6281</v>
+      </c>
+      <c r="B39" t="s">
+        <v>146</v>
+      </c>
+      <c r="C39" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40">
+        <v>6951</v>
+      </c>
+      <c r="B40" t="s">
+        <v>166</v>
+      </c>
+      <c r="C40" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41">
+        <v>50863</v>
+      </c>
+      <c r="B41" t="s">
+        <v>777</v>
+      </c>
+      <c r="C41" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42">
+        <v>97476</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1277</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1278</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43">
+        <v>103730</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1436</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1438</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44">
+        <v>106040</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1397</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45">
+        <v>319201</v>
+      </c>
+      <c r="B45" t="s">
+        <v>855</v>
+      </c>
+      <c r="C45" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46">
+        <v>707549</v>
+      </c>
+      <c r="B46" t="s">
+        <v>873</v>
+      </c>
+      <c r="C46" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47">
+        <v>723125</v>
+      </c>
+      <c r="B47" t="s">
+        <v>964</v>
+      </c>
+      <c r="C47" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48">
+        <v>827054</v>
+      </c>
+      <c r="B48" t="s">
+        <v>961</v>
+      </c>
+      <c r="C48" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49">
+        <v>1819438</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1909</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1910</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50">
+        <v>915913</v>
+      </c>
+      <c r="B50" t="s">
+        <v>61</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1911</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51">
+        <v>1874178</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1912</v>
+      </c>
+      <c r="C51" t="s">
+        <v>1913</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52">
+        <v>1274494</v>
+      </c>
+      <c r="B52" t="s">
+        <v>628</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1914</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53">
+        <v>1318605</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1275</v>
+      </c>
+      <c r="C53" t="s">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54">
+        <v>34088</v>
+      </c>
+      <c r="B54" t="s">
+        <v>603</v>
+      </c>
+      <c r="C54" t="s">
+        <v>1915</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55">
+        <v>93410</v>
+      </c>
+      <c r="B55" t="s">
+        <v>365</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56">
+        <v>1811210</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1917</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57">
+        <v>63908</v>
+      </c>
+      <c r="B57" t="s">
+        <v>942</v>
+      </c>
+      <c r="C57" t="s">
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58">
+        <v>1048911</v>
+      </c>
+      <c r="B58" t="s">
+        <v>620</v>
+      </c>
+      <c r="C58" t="s">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59">
+        <v>1820953</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1922</v>
+      </c>
+      <c r="C59" t="s">
+        <v>1921</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60">
+        <v>354950</v>
+      </c>
+      <c r="B60" t="s">
+        <v>728</v>
+      </c>
+      <c r="C60" t="s">
+        <v>1923</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61">
+        <v>1018724</v>
+      </c>
+      <c r="B61" t="s">
+        <v>96</v>
+      </c>
+      <c r="C61" t="s">
+        <v>1924</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62">
+        <v>66740</v>
+      </c>
+      <c r="B62" t="s">
+        <v>3</v>
+      </c>
+      <c r="C62" t="s">
+        <v>1925</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63">
+        <v>1108524</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1201</v>
+      </c>
+      <c r="C63" t="s">
+        <v>1926</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64">
+        <v>789019</v>
+      </c>
+      <c r="B64" t="s">
+        <v>967</v>
+      </c>
+      <c r="C64" t="s">
+        <v>1927</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65">
+        <v>796343</v>
+      </c>
+      <c r="B65" t="s">
+        <v>26</v>
+      </c>
+      <c r="C65" t="s">
+        <v>1928</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66">
+        <v>909832</v>
+      </c>
+      <c r="B66" t="s">
+        <v>445</v>
+      </c>
+      <c r="C66" t="s">
+        <v>1929</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67">
+        <v>1744489</v>
+      </c>
+      <c r="B67" t="s">
+        <v>1375</v>
+      </c>
+      <c r="C67" t="s">
+        <v>1930</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68">
+        <v>18230</v>
+      </c>
+      <c r="B68" t="s">
+        <v>324</v>
+      </c>
+      <c r="C68" t="s">
+        <v>1931</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69">
+        <v>1650372</v>
+      </c>
+      <c r="B69" t="s">
+        <v>1932</v>
+      </c>
+      <c r="C69" t="s">
+        <v>1933</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70">
+        <v>804328</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C70" t="s">
+        <v>1934</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71">
+        <v>104169</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1372</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1935</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72">
+        <v>1403161</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1359</v>
+      </c>
+      <c r="C72" t="s">
+        <v>1936</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73">
+        <v>1512673</v>
+      </c>
+      <c r="B73" t="s">
+        <v>1937</v>
+      </c>
+      <c r="C73" t="s">
+        <v>1938</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C19" xr:uid="{17146AA1-C78E-482C-A866-46B8415D9924}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C19">
-      <sortCondition ref="A1:A19"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:C1" xr:uid="{17146AA1-C78E-482C-A866-46B8415D9924}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA2DD92A-2E90-4DD2-A757-3ED9B36B3509}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="18" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added feature to run engine with selected company and year
</commit_message>
<xml_diff>
--- a/company_list.xlsx
+++ b/company_list.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\GitHub\hellotaoworld\valuation_engine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tao_project\valuation_engine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3E3E2E-1655-4F29-BC0E-981936AA1E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C51A58-7FE3-4760-B501-FCD6858D78E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31725" yWindow="0" windowWidth="24780" windowHeight="15735" activeTab="2" xr2:uid="{B82EAC9A-0CE0-46BB-ACD0-5E3D12938F59}"/>
+    <workbookView xWindow="32490" yWindow="1020" windowWidth="21600" windowHeight="11385" xr2:uid="{B82EAC9A-0CE0-46BB-ACD0-5E3D12938F59}"/>
   </bookViews>
   <sheets>
     <sheet name="sic" sheetId="3" r:id="rId1"/>
     <sheet name="sp500" sheetId="1" r:id="rId2"/>
     <sheet name="pick" sheetId="2" r:id="rId3"/>
-    <sheet name="checked_pick" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">pick!$A$1:$C$1</definedName>
@@ -90,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3607" uniqueCount="1982">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3604" uniqueCount="1982">
   <si>
     <t>symbol</t>
   </si>
@@ -6544,10 +6543,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86D46672-D027-46D5-9826-3A1061371C59}">
+  <sheetPr>
+    <tabColor theme="9"/>
+  </sheetPr>
   <dimension ref="A1:C445"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11461,9 +11463,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DB4D047-C06A-42FE-BFF0-99FF6773CE7A}">
+  <sheetPr>
+    <tabColor theme="9"/>
+  </sheetPr>
   <dimension ref="A1:G504"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A469" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -23079,13 +23084,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17146AA1-C78E-482C-A866-46B8415D9924}">
+  <sheetPr>
+    <tabColor theme="9"/>
+  </sheetPr>
   <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -23901,33 +23909,4 @@
   <autoFilter ref="A1:C1" xr:uid="{17146AA1-C78E-482C-A866-46B8415D9924}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA2DD92A-2E90-4DD2-A757-3ED9B36B3509}">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C48"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="18" defaultRowHeight="15"/>
-  <cols>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>